<commit_message>
replaced colors between stay and new-comers
</commit_message>
<xml_diff>
--- a/assets/color_labels.xlsx
+++ b/assets/color_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shai/Google Drive offline/Education/Article Publications/population demographic tracking/git/demographic_estimation_dashboard_article/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5501C07A-61DC-8B45-A665-6025BE60C96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4468E6F-868A-E748-99FC-D128F9FFF467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19320" yWindow="500" windowWidth="14280" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -555,7 +555,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -566,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>